<commit_message>
Learning SQL commands, preparing to make structure of program
</commit_message>
<xml_diff>
--- a/Directions.xlsx
+++ b/Directions.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Claire B</t>
   </si>
   <si>
-    <t xml:space="preserve">Put all in a rice cooker or cook quinoa and veggies seperately then add everything together</t>
+    <t xml:space="preserve">Put all in a rice cooker or cook quinoa and veggies separately then add everything together</t>
   </si>
   <si>
     <t xml:space="preserve">Chewy Oatmeal Cookies</t>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">Mitchell B</t>
   </si>
   <si>
-    <t xml:space="preserve">Pour borth in pot, cut up veggies and put in broth, put chicken in broth, bring to boil and put noodles in, season to taste, boil until chicken and noodles cooked, pull apart chicken and put back in soup</t>
+    <t xml:space="preserve">Pour broth in pot, cut up veggies and put in broth, put chicken in broth, bring to boil and put noodles in, season to taste, boil until chicken and noodles cooked, pull apart chicken and put back in soup</t>
   </si>
   <si>
     <t xml:space="preserve">Crustless Quiche</t>
@@ -79,10 +79,10 @@
     <t xml:space="preserve">Mary B</t>
   </si>
   <si>
-    <t xml:space="preserve">Create egg and cream mixture with spices, spray pan, thin walled baking pan preffered. Bake at 325 for 25-30 minutes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zuchinni Bread</t>
+    <t xml:space="preserve">Create egg and cream mixture with spices, spray pan, thin walled baking pan preferred bake at 325 for 25-30 minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zucchini Bread</t>
   </si>
   <si>
     <t xml:space="preserve">TBD</t>
@@ -94,13 +94,13 @@
     <t xml:space="preserve">Shalane F</t>
   </si>
   <si>
-    <t xml:space="preserve">Oven to 400F, baking sheet with parchment paper with oil on top, combine ingreds and let rest for 15 mins, bake for 30 mins, flip halfway thru</t>
+    <t xml:space="preserve">Oven to 400F, baking sheet with parchment paper with oil on top, combine ingredients and let rest for 15 mins, bake for 30 mins, flip halfway thru</t>
   </si>
   <si>
     <t xml:space="preserve">Chipotle Black Bean Burgers</t>
   </si>
   <si>
-    <t xml:space="preserve">Pre cook onions, wash and dy beans, then mix everything in pan and cook with cast iron skillet if possible</t>
+    <t xml:space="preserve">Pre cook onions, wash and dry beans, then mix everything in pan and cook with cast iron skillet if possible</t>
   </si>
   <si>
     <t xml:space="preserve">Honey Balsamic Grilled Chicken</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">Marinate chicken overnight, grill or cook on stove</t>
   </si>
   <si>
-    <t xml:space="preserve">Tempeh Ratatoullie</t>
+    <t xml:space="preserve">Tempeh Ratatouille</t>
   </si>
   <si>
     <t xml:space="preserve">Cook veggies in oil till soft, add chickpeas or tempeh, simmer 25 minutes, add vinegar and pepper at end</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">Chicken and Rice Stew</t>
   </si>
   <si>
-    <t xml:space="preserve">Get large soup pan, cut up veggies and simmer in oil till soft, add broth and chicken simmer for 30 mins, pull apart chicken with forks, return chicken to pot, stir in parsely and spinach and lemon juice</t>
+    <t xml:space="preserve">Get large soup pan, cut up veggies and simmer in oil till soft, add broth and chicken simmer for 30 mins, pull apart chicken with forks, return chicken to pot, stir in parsley and spinach and lemon juice</t>
   </si>
   <si>
     <t xml:space="preserve">Super Hero Muffins</t>
@@ -270,7 +270,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -435,7 +435,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>35</v>
       </c>

</xml_diff>